<commit_message>
[Document, Modified] : TaskList(1) and MyMusic UseCase Specification
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/UseCase/TaskList/TaskList(1) Specification.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/UseCase/TaskList/TaskList(1) Specification.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7830" firstSheet="7" activeTab="7"/>
+    <workbookView windowWidth="19815" windowHeight="7830" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Manage Project" sheetId="9" r:id="rId1"/>
@@ -603,14 +603,13 @@
     <t>Chức năng đánh dấu những task yêu thích</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Người dùng nhấn Task cụ thể
+    <t>- Người dùng nhấn Task cụ thể
  - Hệ thống hiển thị form task 
  - Người dùng nhấn vào biểu tượng Favaorite
- - Hệ thống lưu trạng thái favorite của task dưới CSDL
-</t>
-  </si>
-  <si>
-    <t>- Người dùng nhấn Task cụ thể 
+ - Hệ thống lưu trạng thái favorite của task dưới CSDL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Người dùng nhấn Task cụ thể 
  - Người dùng nhấn vào biểu tượng favorite</t>
   </si>
   <si>
@@ -818,9 +817,22 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -848,8 +860,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -860,36 +897,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -909,39 +916,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -963,7 +939,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -984,7 +983,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -996,43 +1043,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1050,25 +1085,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1080,61 +1151,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1146,25 +1163,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1313,17 +1312,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1332,7 +1336,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1367,35 +1371,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1410,151 +1385,175 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3476,8 +3475,8 @@
   <sheetPr/>
   <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="3"/>
@@ -3622,7 +3621,7 @@
   <sheetPr/>
   <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -3680,7 +3679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" ht="141.75" spans="2:4">
+    <row r="7" ht="146" customHeight="1" spans="2:4">
       <c r="B7" s="2" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
[Document, Modified] : TaskList(1) Specification
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/UseCase/TaskList/TaskList(1) Specification.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/UseCase/TaskList/TaskList(1) Specification.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7830" firstSheet="7" activeTab="8"/>
+    <workbookView windowWidth="19815" windowHeight="7830" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Manage Project" sheetId="9" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="141">
   <si>
     <t>Use-case number:</t>
   </si>
@@ -705,6 +705,9 @@
     <t>Add Website as Task</t>
   </si>
   <si>
+    <t>Chức năng kéo chèn đường dẫn website vào task</t>
+  </si>
+  <si>
     <t xml:space="preserve"> - Người dùng nhấn Task cụ thể
  - Hệ thống hiển thị form người dùng thao tác
  - Người dùng thêm đường dẫn đến website vào task
@@ -768,9 +771,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -818,13 +821,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
@@ -832,7 +828,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -860,9 +864,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -873,6 +876,30 @@
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -892,32 +919,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -939,7 +942,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -955,14 +965,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -983,48 +986,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1037,7 +998,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1055,13 +1118,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1073,79 +1130,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1163,7 +1148,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1312,6 +1315,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1323,20 +1341,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1352,6 +1359,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1386,33 +1402,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1433,127 +1436,127 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1892,7 +1895,7 @@
   </sheetPr>
   <dimension ref="A2:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2216,7 +2219,7 @@
   <dimension ref="B2:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="3"/>
@@ -2258,7 +2261,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -2275,13 +2278,13 @@
     </row>
     <row r="7" ht="157.5" spans="2:4">
       <c r="B7" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" ht="32" customHeight="1" spans="2:4">
@@ -2307,7 +2310,7 @@
         <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D10" s="2"/>
     </row>
@@ -2316,7 +2319,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -2325,7 +2328,7 @@
         <v>28</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -2334,7 +2337,7 @@
         <v>30</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D13" s="2"/>
     </row>
@@ -2361,7 +2364,7 @@
   <sheetPr/>
   <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -2386,7 +2389,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -2404,7 +2407,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -2421,13 +2424,13 @@
     </row>
     <row r="7" ht="157.5" spans="2:4">
       <c r="B7" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" ht="32" customHeight="1" spans="2:4">
@@ -2462,7 +2465,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -2471,7 +2474,7 @@
         <v>28</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -2480,7 +2483,7 @@
         <v>30</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D13" s="2"/>
     </row>
@@ -3329,7 +3332,7 @@
   <sheetPr/>
   <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -3533,7 +3536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" ht="94.5" spans="2:4">
+    <row r="7" ht="78.75" spans="2:4">
       <c r="B7" s="2" t="s">
         <v>103</v>
       </c>
@@ -3621,7 +3624,7 @@
   <sheetPr/>
   <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[Add, Document] : ManagementTask Specification
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/UseCase/TaskList/TaskList(1) Specification.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/UseCase/TaskList/TaskList(1) Specification.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7830" firstSheet="7" activeTab="11"/>
+    <workbookView windowWidth="19815" windowHeight="7830" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Manage Project" sheetId="9" r:id="rId1"/>
@@ -770,10 +770,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -821,35 +821,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -864,26 +835,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -896,8 +852,44 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -920,7 +912,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -933,16 +941,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -950,14 +958,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -986,7 +986,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -998,13 +1040,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1022,7 +1124,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1034,139 +1166,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1315,21 +1315,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1342,8 +1327,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1363,11 +1348,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1387,17 +1378,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1415,148 +1415,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2364,7 +2364,7 @@
   <sheetPr/>
   <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -2512,7 +2512,7 @@
   </sheetPr>
   <dimension ref="B2:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -2769,7 +2769,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" ht="141.75" spans="2:4">
+    <row r="10" ht="157.5" spans="2:4">
       <c r="B10" s="13"/>
       <c r="C10" s="14" t="s">
         <v>54</v>
@@ -3536,7 +3536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" ht="78.75" spans="2:4">
+    <row r="7" ht="94.5" spans="2:4">
       <c r="B7" s="2" t="s">
         <v>103</v>
       </c>

</xml_diff>